<commit_message>
Testing Reboot Retry method
</commit_message>
<xml_diff>
--- a/TestData/STG_RebootTestData.xlsx
+++ b/TestData/STG_RebootTestData.xlsx
@@ -79,7 +79,7 @@
     <t xml:space="preserve">InsightModelsID</t>
   </si>
   <si>
-    <t xml:space="preserve">1000193599</t>
+    <t xml:space="preserve">10001935991</t>
   </si>
   <si>
     <t xml:space="preserve">1000193627</t>
@@ -233,7 +233,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.03125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>

</xml_diff>